<commit_message>
adding remaining commits from last hw
</commit_message>
<xml_diff>
--- a/a.xlsx
+++ b/a.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="0" windowWidth="25360" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="a.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,10 +31,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -57,13 +80,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -393,13 +437,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B99"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -407,7 +457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>6</v>
       </c>
@@ -415,407 +465,725 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>9</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3">
+        <f>TTEST(A2:A49,A50:A99,1,3)</f>
+        <v>3.9994616114744673E-9</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1">
+        <v>115</v>
+      </c>
+      <c r="I3">
+        <f>TTEST(G3:G50,H3:H52,1,3)</f>
+        <v>3.9994616114744673E-9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="G4">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>33</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>7</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="D6">
+        <f>SUM(A2:A49)</f>
+        <v>865</v>
+      </c>
+      <c r="E6">
+        <f>AVERAGE(B2:B49)</f>
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>33</v>
+      </c>
+      <c r="H6" s="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="D7">
+        <f>SUM(A50:A99)</f>
+        <v>4400</v>
+      </c>
+      <c r="E7">
+        <f>AVERAGE(A50:A99)</f>
+        <v>88</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="H7" s="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>26</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>17</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="G11">
+        <v>26</v>
+      </c>
+      <c r="H11" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>7</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="G12">
+        <v>17</v>
+      </c>
+      <c r="H12" s="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>8</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>11</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>8</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="G15">
+        <v>11</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>8</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>7</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="G18">
+        <v>17</v>
+      </c>
+      <c r="H18" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>5</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="H19" s="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>7</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>5</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="H21" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>68</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>29</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="G23">
+        <v>68</v>
+      </c>
+      <c r="H23" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>32</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="G24">
+        <v>29</v>
+      </c>
+      <c r="H24" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>43</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="G25">
+        <v>32</v>
+      </c>
+      <c r="H25" s="1">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>9</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="G26">
+        <v>43</v>
+      </c>
+      <c r="H26" s="1">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>10</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="G27">
+        <v>9</v>
+      </c>
+      <c r="H27" s="1">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>5</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="G28">
+        <v>10</v>
+      </c>
+      <c r="H28" s="1">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>30</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="G30">
+        <v>4</v>
+      </c>
+      <c r="H30" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>43</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>5</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="G32">
+        <v>43</v>
+      </c>
+      <c r="H32" s="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>6</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="G33">
+        <v>5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>8</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="G34">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>10</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="G35">
+        <v>8</v>
+      </c>
+      <c r="H35" s="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>65</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>15</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="G37">
+        <v>65</v>
+      </c>
+      <c r="H37" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>15</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="G38">
+        <v>15</v>
+      </c>
+      <c r="H38" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>20</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="G39">
+        <v>15</v>
+      </c>
+      <c r="H39" s="1">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>11</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="G40">
+        <v>20</v>
+      </c>
+      <c r="H40" s="1">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>85</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="G41">
+        <v>11</v>
+      </c>
+      <c r="H41" s="1">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>43</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="G42">
+        <v>85</v>
+      </c>
+      <c r="H42" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>4</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="G43">
+        <v>43</v>
+      </c>
+      <c r="H43" s="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>3</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="G44">
+        <v>4</v>
+      </c>
+      <c r="H44" s="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>52</v>
       </c>
       <c r="B46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>26</v>
       </c>
       <c r="B47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="G47">
+        <v>52</v>
+      </c>
+      <c r="H47" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>5</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="G48">
+        <v>26</v>
+      </c>
+      <c r="H48" s="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>7</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="G49">
+        <v>5</v>
+      </c>
+      <c r="H49" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>115</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="G50">
+        <v>7</v>
+      </c>
+      <c r="H50" s="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>57</v>
       </c>
       <c r="B51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="H51" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>2</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="H52" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>147</v>
       </c>
@@ -823,7 +1191,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>113</v>
       </c>
@@ -831,7 +1199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>100</v>
       </c>
@@ -839,7 +1207,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>1</v>
       </c>
@@ -847,7 +1215,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>49</v>
       </c>
@@ -855,7 +1223,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>2</v>
       </c>
@@ -863,7 +1231,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>119</v>
       </c>
@@ -871,7 +1239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>125</v>
       </c>
@@ -879,7 +1247,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>2</v>
       </c>
@@ -887,7 +1255,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>1</v>
       </c>
@@ -895,7 +1263,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>132</v>
       </c>
@@ -903,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>128</v>
       </c>
@@ -1193,6 +1561,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>